<commit_message>
EPBDS-9610 Cyrillic symbols test was added. Validation of the table names for UI was changed.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9610-special_symbols_in_names.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9610-special_symbols_in_names.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DCBA6B-2427-4147-A966-EBC3D1F287FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0403B5-47F0-46EC-A37B-9C396BB4F366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15840" xr2:uid="{19718910-8F54-4705-937E-9DD2C8098F4C}"/>
+    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15225" activeTab="1" xr2:uid="{19718910-8F54-4705-937E-9DD2C8098F4C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="invalidNames" sheetId="1" r:id="rId1"/>
+    <sheet name="validCyrillic" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="63">
   <si>
     <t>String</t>
   </si>
@@ -222,12 +223,65 @@
       <t>?a</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+      </rPr>
+      <t>Datatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> мойДататип</t>
+    </r>
+  </si>
+  <si>
+    <t>Spreadsheet Integer мойМетод(Integer a)</t>
+  </si>
+  <si>
+    <t>Test  мойМетод мойТест</t>
+  </si>
+  <si>
+    <t>Properties моиПроперти</t>
+  </si>
+  <si>
+    <t>Constants постояннаяПланка</t>
+  </si>
+  <si>
+    <t>Conditions условия</t>
+  </si>
+  <si>
+    <t>Conditions ещеОдниусловия</t>
+  </si>
+  <si>
+    <t>Returns таблица</t>
+  </si>
+  <si>
+    <t>Returns ещеОднаТаблица</t>
+  </si>
+  <si>
+    <t>Actions действия</t>
+  </si>
+  <si>
+    <t>Data мойДататип дата</t>
+  </si>
+  <si>
+    <t>Datatype дататип123 &lt;String&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +326,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -414,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -463,6 +523,17 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -505,6 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1 10" xfId="1" xr:uid="{5FEDD8BE-38D5-4A35-A69E-4A249C55A0BA}"/>
@@ -822,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C93270-DBF9-42A3-B7CA-FEC9A939D06A}">
   <dimension ref="B3:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -832,10 +904,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="40"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
@@ -846,9 +918,9 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
@@ -901,10 +973,10 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="36"/>
+      <c r="C20" s="41"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="2" t="s">
@@ -948,14 +1020,14 @@
       <c r="B26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="31" t="s">
+      <c r="H26" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="33"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="38"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="2" t="s">
@@ -964,10 +1036,10 @@
       <c r="H27" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I27" s="27" t="s">
+      <c r="I27" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="J27" s="27"/>
+      <c r="J27" s="32"/>
       <c r="K27" s="4" t="s">
         <v>39</v>
       </c>
@@ -983,42 +1055,42 @@
       <c r="H28" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="27" t="s">
+      <c r="I28" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27" t="s">
+      <c r="J28" s="32"/>
+      <c r="K28" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="L28" s="27"/>
-      <c r="M28" s="28" t="s">
+      <c r="L28" s="32"/>
+      <c r="M28" s="33" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="H29" s="16"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="28"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="33"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
       <c r="H30" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="27" t="s">
+      <c r="I30" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="28" t="s">
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="33" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1033,42 +1105,42 @@
         <v>19</v>
       </c>
       <c r="H31" s="16"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="28"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="33"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="H32" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="27" t="s">
+      <c r="I32" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="28" t="s">
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="33" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="37" t="s">
+      <c r="C33" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="37" t="s">
+      <c r="D33" s="42" t="s">
         <v>21</v>
       </c>
       <c r="H33" s="16"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="28"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="33"/>
     </row>
     <row r="34" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B34" s="3" t="s">
@@ -1081,11 +1153,11 @@
         <v>23</v>
       </c>
       <c r="H34" s="17"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="29"/>
-      <c r="M34" s="30"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="35"/>
     </row>
     <row r="35" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="36" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -1109,35 +1181,35 @@
       <c r="E37" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H37" s="31" t="s">
+      <c r="H37" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="33"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="38"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="29" t="s">
         <v>29</v>
       </c>
       <c r="H38" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I38" s="27" t="s">
+      <c r="I38" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="J38" s="27"/>
+      <c r="J38" s="32"/>
       <c r="K38" s="4" t="s">
         <v>39</v>
       </c>
@@ -1147,114 +1219,114 @@
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B39" s="21"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="24"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="29"/>
       <c r="H39" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I39" s="27" t="s">
+      <c r="I39" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27" t="s">
+      <c r="J39" s="32"/>
+      <c r="K39" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="L39" s="27"/>
-      <c r="M39" s="28" t="s">
+      <c r="L39" s="32"/>
+      <c r="M39" s="33" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="23"/>
-      <c r="E40" s="24" t="s">
+      <c r="D40" s="28"/>
+      <c r="E40" s="29" t="s">
         <v>33</v>
       </c>
       <c r="H40" s="16"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="28"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
+      <c r="L40" s="32"/>
+      <c r="M40" s="33"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B41" s="21"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="24"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="29"/>
       <c r="H41" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I41" s="27" t="s">
+      <c r="I41" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="28" t="s">
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="32"/>
+      <c r="M41" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D42" s="23"/>
-      <c r="E42" s="24"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="29"/>
       <c r="H42" s="16"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="28"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="33"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43" s="21"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="24"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="29"/>
       <c r="H43" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I43" s="27" t="s">
+      <c r="I43" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="28" t="s">
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="33" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B44" s="22"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="26"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="31"/>
       <c r="H44" s="16"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="28"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="33"/>
     </row>
     <row r="45" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="H45" s="17"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="30"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="35"/>
     </row>
     <row r="46" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B46" s="5" t="s">
@@ -1285,16 +1357,16 @@
       <c r="K47" s="7"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="23" t="s">
+      <c r="C48" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D48" s="23" t="s">
+      <c r="D48" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E48" s="24" t="s">
+      <c r="E48" s="29" t="s">
         <v>29</v>
       </c>
       <c r="H48" s="11" t="s">
@@ -1311,98 +1383,98 @@
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="21"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="24"/>
-      <c r="H49" s="21" t="s">
+      <c r="B49" s="26"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="29"/>
+      <c r="H49" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="I49" s="23" t="s">
+      <c r="I49" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="J49" s="23" t="s">
+      <c r="J49" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="K49" s="24" t="s">
+      <c r="K49" s="29" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="23" t="s">
+      <c r="C50" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D50" s="23"/>
-      <c r="E50" s="24" t="s">
+      <c r="D50" s="28"/>
+      <c r="E50" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="H50" s="21"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="24"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28"/>
+      <c r="K50" s="29"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="21"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="24"/>
-      <c r="H51" s="21" t="s">
+      <c r="B51" s="26"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="29"/>
+      <c r="H51" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="I51" s="23" t="s">
+      <c r="I51" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J51" s="23"/>
-      <c r="K51" s="24" t="s">
+      <c r="J51" s="28"/>
+      <c r="K51" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C52" s="23" t="s">
+      <c r="C52" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D52" s="23"/>
-      <c r="E52" s="24"/>
-      <c r="H52" s="21"/>
-      <c r="I52" s="23"/>
-      <c r="J52" s="23"/>
-      <c r="K52" s="24"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="29"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="29"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53" s="21"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="24"/>
-      <c r="H53" s="21" t="s">
+      <c r="B53" s="26"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="29"/>
+      <c r="H53" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="I53" s="23" t="s">
+      <c r="I53" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="J53" s="23"/>
-      <c r="K53" s="24"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="29"/>
     </row>
     <row r="54" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B54" s="22"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="26"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="23"/>
-      <c r="K54" s="24"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="31"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="29"/>
     </row>
     <row r="55" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="H55" s="22"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="26"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="30"/>
+      <c r="J55" s="30"/>
+      <c r="K55" s="31"/>
     </row>
     <row r="56" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="57" spans="2:11" x14ac:dyDescent="0.55000000000000004">
@@ -1428,64 +1500,64 @@
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H59" s="21" t="s">
+      <c r="H59" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="I59" s="23" t="s">
+      <c r="I59" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="J59" s="23" t="s">
+      <c r="J59" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="K59" s="24" t="s">
+      <c r="K59" s="29" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H60" s="21"/>
-      <c r="I60" s="23"/>
-      <c r="J60" s="23"/>
-      <c r="K60" s="24"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="28"/>
+      <c r="J60" s="28"/>
+      <c r="K60" s="29"/>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H61" s="21" t="s">
+      <c r="H61" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="I61" s="23" t="s">
+      <c r="I61" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J61" s="23"/>
-      <c r="K61" s="24" t="s">
+      <c r="J61" s="28"/>
+      <c r="K61" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H62" s="21"/>
-      <c r="I62" s="23"/>
-      <c r="J62" s="23"/>
-      <c r="K62" s="24"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="28"/>
+      <c r="K62" s="29"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H63" s="21" t="s">
+      <c r="H63" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="I63" s="23" t="s">
+      <c r="I63" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="J63" s="23"/>
-      <c r="K63" s="24"/>
+      <c r="J63" s="28"/>
+      <c r="K63" s="29"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H64" s="21"/>
-      <c r="I64" s="23"/>
-      <c r="J64" s="23"/>
-      <c r="K64" s="24"/>
+      <c r="H64" s="26"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="28"/>
+      <c r="K64" s="29"/>
     </row>
     <row r="65" spans="8:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="H65" s="22"/>
-      <c r="I65" s="25"/>
-      <c r="J65" s="25"/>
-      <c r="K65" s="26"/>
+      <c r="H65" s="27"/>
+      <c r="I65" s="30"/>
+      <c r="J65" s="30"/>
+      <c r="K65" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="59">
@@ -1551,4 +1623,1091 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC80BC21-61C2-4A25-BA80-816F28108965}">
+  <dimension ref="B3:N56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="24">
+        <v>2</v>
+      </c>
+      <c r="C19" s="24">
+        <v>3</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="41"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+    </row>
+    <row r="26" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="24"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="J28" s="32"/>
+      <c r="K28" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L28" s="24"/>
+      <c r="M28" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28" s="24"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="L29" s="32"/>
+      <c r="M29" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="N29" s="24"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="24"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="N31" s="24"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="24"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="N33" s="24"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="24"/>
+    </row>
+    <row r="35" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B35" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="34"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="24"/>
+    </row>
+    <row r="36" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="24"/>
+    </row>
+    <row r="37" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="38"/>
+      <c r="N38" s="24"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="J39" s="32"/>
+      <c r="K39" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L39" s="24"/>
+      <c r="M39" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N39" s="24"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="26"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="32"/>
+      <c r="M40" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="N40" s="24"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="28"/>
+      <c r="E41" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="32"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="24"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" s="26"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I42" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="N42" s="24"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="28"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="24"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" s="26"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I44" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="N44" s="24"/>
+    </row>
+    <row r="45" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B45" s="27"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="33"/>
+      <c r="N45" s="24"/>
+    </row>
+    <row r="46" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="34"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="24"/>
+    </row>
+    <row r="47" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B47" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="24"/>
+      <c r="M47" s="24"/>
+      <c r="N47" s="24"/>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="24"/>
+      <c r="M48" s="24"/>
+      <c r="N48" s="24"/>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I49" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="J49" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="K49" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="L49" s="24"/>
+      <c r="M49" s="24"/>
+      <c r="N49" s="24"/>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" s="26"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I50" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="J50" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="K50" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="L50" s="24"/>
+      <c r="M50" s="24"/>
+      <c r="N50" s="24"/>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="28"/>
+      <c r="E51" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="28"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="24"/>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" s="26"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="I52" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="J52" s="28"/>
+      <c r="K52" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="L52" s="24"/>
+      <c r="M52" s="24"/>
+      <c r="N52" s="24"/>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="28"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="29"/>
+      <c r="L53" s="24"/>
+      <c r="M53" s="24"/>
+      <c r="N53" s="24"/>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" s="26"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="I54" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="J54" s="28"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="24"/>
+      <c r="M54" s="24"/>
+      <c r="N54" s="24"/>
+    </row>
+    <row r="55" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B55" s="27"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="28"/>
+      <c r="J55" s="28"/>
+      <c r="K55" s="29"/>
+      <c r="L55" s="24"/>
+      <c r="M55" s="24"/>
+      <c r="N55" s="24"/>
+    </row>
+    <row r="56" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="30"/>
+      <c r="J56" s="30"/>
+      <c r="K56" s="31"/>
+      <c r="L56" s="24"/>
+      <c r="M56" s="24"/>
+      <c r="N56" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="50">
+    <mergeCell ref="I29:J30"/>
+    <mergeCell ref="K29:L30"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="I31:L32"/>
+    <mergeCell ref="M31:M32"/>
+    <mergeCell ref="I33:L35"/>
+    <mergeCell ref="M33:M35"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I40:J41"/>
+    <mergeCell ref="K40:L41"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:E45"/>
+    <mergeCell ref="I44:L46"/>
+    <mergeCell ref="M44:M46"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="I50:I51"/>
+    <mergeCell ref="C41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="I42:L43"/>
+    <mergeCell ref="H54:H56"/>
+    <mergeCell ref="I54:K56"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="K50:K51"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="H52:H53"/>
+    <mergeCell ref="I52:J53"/>
+    <mergeCell ref="K52:K53"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:E55"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-9610 warnings usage. This commit must be reverted in 5.24 branch
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9610-special_symbols_in_names.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9610-special_symbols_in_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0403B5-47F0-46EC-A37B-9C396BB4F366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058CDDBB-933B-46C4-AEB7-111E65507570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15225" activeTab="1" xr2:uid="{19718910-8F54-4705-937E-9DD2C8098F4C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="62">
   <si>
     <t>String</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>POLICYID</t>
-  </si>
-  <si>
-    <t>Data 2m da/?tat</t>
   </si>
   <si>
     <t>Double</t>
@@ -250,9 +247,6 @@
     <t>Test  мойМетод мойТест</t>
   </si>
   <si>
-    <t>Properties моиПроперти</t>
-  </si>
-  <si>
     <t>Constants постояннаяПланка</t>
   </si>
   <si>
@@ -275,6 +269,9 @@
   </si>
   <si>
     <t>Datatype дататип123 &lt;String&gt;</t>
+  </si>
+  <si>
+    <t>Data 2m?a da/?tat</t>
   </si>
 </sst>
 </file>
@@ -366,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -469,12 +466,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -531,6 +565,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -577,6 +614,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1 10" xfId="1" xr:uid="{5FEDD8BE-38D5-4A35-A69E-4A249C55A0BA}"/>
@@ -894,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C93270-DBF9-42A3-B7CA-FEC9A939D06A}">
   <dimension ref="B3:M65"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -904,10 +952,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="40"/>
+      <c r="B3" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="41"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
@@ -918,9 +966,9 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
@@ -973,10 +1021,10 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="41"/>
+      <c r="C20" s="42"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="2" t="s">
@@ -1018,34 +1066,34 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="38"/>
+        <v>61</v>
+      </c>
+      <c r="H26" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="39"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="33"/>
+      <c r="K27" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="J27" s="32"/>
-      <c r="K27" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.55000000000000004">
@@ -1053,116 +1101,116 @@
         <v>15</v>
       </c>
       <c r="H28" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="32" t="s">
+      <c r="J28" s="33"/>
+      <c r="K28" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="L28" s="32"/>
-      <c r="M28" s="33" t="s">
-        <v>29</v>
+      <c r="L28" s="33"/>
+      <c r="M28" s="34" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="H29" s="16"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="34"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
+      <c r="B30" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
       <c r="H30" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="33" t="s">
-        <v>41</v>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="34" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="H31" s="16"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="34"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="H32" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I32" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="33" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="42" t="s">
-        <v>21</v>
+      <c r="B33" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="43" t="s">
+        <v>20</v>
       </c>
       <c r="H33" s="16"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="34"/>
     </row>
     <row r="34" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B34" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="H34" s="17"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="36"/>
     </row>
     <row r="35" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="36" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B36" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -1170,167 +1218,167 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="D37" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="E37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="39"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H37" s="36" t="s">
+      <c r="C38" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="38"/>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B38" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="H38" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I38" s="32" t="s">
+      <c r="J38" s="33"/>
+      <c r="K38" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="J38" s="32"/>
-      <c r="K38" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" s="27"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="30"/>
+      <c r="H39" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I39" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="L39" s="33"/>
+      <c r="M39" s="34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="29"/>
+      <c r="E40" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H40" s="16"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="34"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" s="27"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="30"/>
+      <c r="H41" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I41" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B39" s="26"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="29"/>
-      <c r="H39" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32" t="s">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="29"/>
+      <c r="E42" s="30"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="34"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" s="27"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="30"/>
+      <c r="H43" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="L39" s="32"/>
-      <c r="M39" s="33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B40" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" s="28"/>
-      <c r="E40" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="H40" s="16"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="33"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B41" s="26"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="29"/>
-      <c r="H41" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I41" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="33" t="s">
+      <c r="I43" s="33" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="28"/>
-      <c r="E42" s="29"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="33"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43" s="26"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="29"/>
-      <c r="H43" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I43" s="32" t="s">
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="33" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="44" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B44" s="27"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="31"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="32"/>
       <c r="H44" s="16"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="34"/>
     </row>
     <row r="45" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="H45" s="17"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
-      <c r="K45" s="34"/>
-      <c r="L45" s="34"/>
-      <c r="M45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="36"/>
     </row>
     <row r="46" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B46" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -1338,148 +1386,148 @@
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="D47" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D47" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="E47" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="7"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="D48" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D48" s="28" t="s">
+      <c r="E48" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K48" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" s="27"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="30"/>
+      <c r="H49" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I49" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="J49" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="K49" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E48" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I48" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="J48" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="K48" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="26"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="29"/>
-      <c r="H49" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="I49" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="J49" s="28" t="s">
+      <c r="C50" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="29"/>
+      <c r="E50" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H50" s="27"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="30"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" s="27"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="30"/>
+      <c r="H51" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="K49" s="29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B50" s="26" t="s">
+      <c r="I51" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="28" t="s">
+      <c r="J51" s="29"/>
+      <c r="K51" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D50" s="28"/>
-      <c r="E50" s="29" t="s">
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="H50" s="26"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
-      <c r="K50" s="29"/>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="26"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="29"/>
-      <c r="H51" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="I51" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="J51" s="28"/>
-      <c r="K51" s="29" t="s">
+      <c r="C52" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="29"/>
+      <c r="E52" s="30"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="30"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" s="27"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="30"/>
+      <c r="H53" s="27" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B52" s="26" t="s">
+      <c r="I53" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C52" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D52" s="28"/>
-      <c r="E52" s="29"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="28"/>
-      <c r="J52" s="28"/>
-      <c r="K52" s="29"/>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53" s="26"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="29"/>
-      <c r="H53" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="I53" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="J53" s="28"/>
-      <c r="K53" s="29"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="30"/>
     </row>
     <row r="54" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B54" s="27"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="31"/>
-      <c r="H54" s="26"/>
-      <c r="I54" s="28"/>
-      <c r="J54" s="28"/>
-      <c r="K54" s="29"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="32"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="30"/>
     </row>
     <row r="55" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="H55" s="27"/>
-      <c r="I55" s="30"/>
-      <c r="J55" s="30"/>
-      <c r="K55" s="31"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="31"/>
+      <c r="K55" s="32"/>
     </row>
     <row r="56" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="57" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="H57" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
@@ -1487,77 +1535,77 @@
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="H58" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I58" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J58" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="J58" s="19" t="s">
+      <c r="K58" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="K58" s="20" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H59" s="26" t="s">
+      <c r="H59" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I59" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="I59" s="28" t="s">
+      <c r="J59" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="J59" s="28" t="s">
+      <c r="K59" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H60" s="27"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="30"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H61" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="K59" s="29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H60" s="26"/>
-      <c r="I60" s="28"/>
-      <c r="J60" s="28"/>
-      <c r="K60" s="29"/>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H61" s="26" t="s">
+      <c r="I61" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="I61" s="28" t="s">
+      <c r="J61" s="29"/>
+      <c r="K61" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="J61" s="28"/>
-      <c r="K61" s="29" t="s">
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H62" s="27"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="29"/>
+      <c r="K62" s="30"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H63" s="27" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H62" s="26"/>
-      <c r="I62" s="28"/>
-      <c r="J62" s="28"/>
-      <c r="K62" s="29"/>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H63" s="26" t="s">
+      <c r="I63" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I63" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="J63" s="28"/>
-      <c r="K63" s="29"/>
+      <c r="J63" s="29"/>
+      <c r="K63" s="30"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H64" s="26"/>
-      <c r="I64" s="28"/>
-      <c r="J64" s="28"/>
-      <c r="K64" s="29"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="29"/>
+      <c r="J64" s="29"/>
+      <c r="K64" s="30"/>
     </row>
     <row r="65" spans="8:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="H65" s="27"/>
-      <c r="I65" s="30"/>
-      <c r="J65" s="30"/>
-      <c r="K65" s="31"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="31"/>
+      <c r="K65" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="59">
@@ -1629,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC80BC21-61C2-4A25-BA80-816F28108965}">
   <dimension ref="B3:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1651,10 +1699,10 @@
       <c r="N3" s="24"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="40"/>
+      <c r="B4" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="41"/>
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
       <c r="F4" s="24"/>
@@ -1732,9 +1780,9 @@
       <c r="N8" s="24"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
@@ -1748,7 +1796,7 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -1848,7 +1896,7 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
@@ -1936,10 +1984,8 @@
       <c r="N20" s="24"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="41"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
@@ -1953,12 +1999,8 @@
       <c r="N21" s="24"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>12</v>
-      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
@@ -1988,7 +2030,7 @@
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
@@ -2037,21 +2079,21 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="38"/>
+      <c r="H27" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="39"/>
       <c r="N27" s="24"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -2064,18 +2106,18 @@
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
       <c r="H28" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" s="33"/>
+      <c r="K28" s="24" t="s">
         <v>38</v>
-      </c>
-      <c r="J28" s="32"/>
-      <c r="K28" s="24" t="s">
-        <v>39</v>
       </c>
       <c r="L28" s="24"/>
       <c r="M28" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N28" s="24"/>
     </row>
@@ -2089,18 +2131,18 @@
       <c r="F29" s="24"/>
       <c r="G29" s="24"/>
       <c r="H29" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="32" t="s">
+      <c r="J29" s="33"/>
+      <c r="K29" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="L29" s="32"/>
-      <c r="M29" s="33" t="s">
-        <v>29</v>
+      <c r="L29" s="33"/>
+      <c r="M29" s="34" t="s">
+        <v>28</v>
       </c>
       <c r="N29" s="24"/>
     </row>
@@ -2112,55 +2154,55 @@
       <c r="F30" s="24"/>
       <c r="G30" s="24"/>
       <c r="H30" s="16"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="34"/>
       <c r="N30" s="24"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
+      <c r="B31" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="48"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
       <c r="H31" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="I31" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="33" t="s">
-        <v>41</v>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="N31" s="24"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="D32" s="25" t="s">
         <v>18</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>19</v>
       </c>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
       <c r="G32" s="24"/>
       <c r="H32" s="16"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="34"/>
       <c r="N32" s="24"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -2171,59 +2213,59 @@
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
       <c r="H33" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I33" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="33" t="s">
-        <v>43</v>
-      </c>
       <c r="N33" s="24"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="42" t="s">
-        <v>21</v>
+      <c r="B34" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
       <c r="H34" s="16"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="34"/>
       <c r="N34" s="24"/>
     </row>
     <row r="35" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B35" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="25" t="s">
         <v>22</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>23</v>
       </c>
       <c r="E35" s="24"/>
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
       <c r="H35" s="17"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="34"/>
-      <c r="M35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="36"/>
       <c r="N35" s="24"/>
     </row>
     <row r="36" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2243,7 +2285,7 @@
     </row>
     <row r="37" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B37" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -2260,178 +2302,178 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="D38" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="22" t="s">
-        <v>27</v>
-      </c>
       <c r="E38" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F38" s="24"/>
       <c r="G38" s="24"/>
-      <c r="H38" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="38"/>
+      <c r="H38" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="39"/>
       <c r="N38" s="24"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="D39" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>29</v>
+      <c r="E39" s="30" t="s">
+        <v>28</v>
       </c>
       <c r="F39" s="24"/>
       <c r="G39" s="24"/>
       <c r="H39" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I39" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="J39" s="33"/>
+      <c r="K39" s="24" t="s">
         <v>38</v>
-      </c>
-      <c r="J39" s="32"/>
-      <c r="K39" s="24" t="s">
-        <v>39</v>
       </c>
       <c r="L39" s="24"/>
       <c r="M39" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N39" s="24"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B40" s="26"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="29"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="30"/>
       <c r="F40" s="24"/>
       <c r="G40" s="24"/>
       <c r="H40" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I40" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="I40" s="32" t="s">
+      <c r="J40" s="33"/>
+      <c r="K40" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32" t="s">
+      <c r="L40" s="33"/>
+      <c r="M40" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="N40" s="24"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="L40" s="32"/>
-      <c r="M40" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="N40" s="24"/>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B41" s="26" t="s">
+      <c r="C41" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="D41" s="29"/>
+      <c r="E41" s="30" t="s">
         <v>32</v>
-      </c>
-      <c r="D41" s="28"/>
-      <c r="E41" s="29" t="s">
-        <v>33</v>
       </c>
       <c r="F41" s="24"/>
       <c r="G41" s="24"/>
       <c r="H41" s="16"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="34"/>
       <c r="N41" s="24"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="26"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="29"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="30"/>
       <c r="F42" s="24"/>
       <c r="G42" s="24"/>
       <c r="H42" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I42" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="I42" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="33" t="s">
-        <v>41</v>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="N42" s="24"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="28"/>
-      <c r="E43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="30"/>
       <c r="F43" s="24"/>
       <c r="G43" s="24"/>
       <c r="H43" s="16"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="34"/>
       <c r="N43" s="24"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B44" s="26"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="29"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="30"/>
       <c r="F44" s="24"/>
       <c r="G44" s="24"/>
       <c r="H44" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I44" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="I44" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="J44" s="33"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="33" t="s">
-        <v>43</v>
-      </c>
       <c r="N44" s="24"/>
     </row>
     <row r="45" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B45" s="27"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="31"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="32"/>
       <c r="F45" s="24"/>
       <c r="G45" s="24"/>
       <c r="H45" s="16"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="34"/>
       <c r="N45" s="24"/>
     </row>
     <row r="46" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2442,16 +2484,16 @@
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
       <c r="H46" s="17"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="34"/>
-      <c r="M46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="36"/>
       <c r="N46" s="24"/>
     </row>
     <row r="47" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B47" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -2468,21 +2510,21 @@
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="D48" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D48" s="22" t="s">
-        <v>27</v>
-      </c>
       <c r="E48" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
       <c r="H48" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
@@ -2492,150 +2534,150 @@
       <c r="N48" s="24"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="28" t="s">
+      <c r="D49" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D49" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" s="29" t="s">
-        <v>29</v>
+      <c r="E49" s="30" t="s">
+        <v>28</v>
       </c>
       <c r="F49" s="24"/>
       <c r="G49" s="24"/>
       <c r="H49" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I49" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="J49" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="J49" s="22" t="s">
+      <c r="K49" s="23" t="s">
         <v>46</v>
-      </c>
-      <c r="K49" s="23" t="s">
-        <v>47</v>
       </c>
       <c r="L49" s="24"/>
       <c r="M49" s="24"/>
       <c r="N49" s="24"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B50" s="26"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="29"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="30"/>
       <c r="F50" s="24"/>
       <c r="G50" s="24"/>
-      <c r="H50" s="26" t="s">
+      <c r="H50" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I50" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="I50" s="28" t="s">
+      <c r="J50" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="J50" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="K50" s="29" t="s">
-        <v>29</v>
+      <c r="K50" s="30" t="s">
+        <v>28</v>
       </c>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
       <c r="N50" s="24"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="28" t="s">
+      <c r="D51" s="29"/>
+      <c r="E51" s="30" t="s">
         <v>32</v>
-      </c>
-      <c r="D51" s="28"/>
-      <c r="E51" s="29" t="s">
-        <v>33</v>
       </c>
       <c r="F51" s="24"/>
       <c r="G51" s="24"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="28"/>
-      <c r="J51" s="28"/>
-      <c r="K51" s="29"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="30"/>
       <c r="L51" s="24"/>
       <c r="M51" s="24"/>
       <c r="N51" s="24"/>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B52" s="26"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="29"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="30"/>
       <c r="F52" s="24"/>
       <c r="G52" s="24"/>
-      <c r="H52" s="26" t="s">
+      <c r="H52" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I52" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="I52" s="28" t="s">
+      <c r="J52" s="29"/>
+      <c r="K52" s="30" t="s">
         <v>32</v>
-      </c>
-      <c r="J52" s="28"/>
-      <c r="K52" s="29" t="s">
-        <v>33</v>
       </c>
       <c r="L52" s="24"/>
       <c r="M52" s="24"/>
       <c r="N52" s="24"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53" s="26" t="s">
+      <c r="B53" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D53" s="28"/>
-      <c r="E53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="30"/>
       <c r="F53" s="24"/>
       <c r="G53" s="24"/>
-      <c r="H53" s="26"/>
-      <c r="I53" s="28"/>
-      <c r="J53" s="28"/>
-      <c r="K53" s="29"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="30"/>
       <c r="L53" s="24"/>
       <c r="M53" s="24"/>
       <c r="N53" s="24"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B54" s="26"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="29"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="30"/>
       <c r="F54" s="24"/>
       <c r="G54" s="24"/>
-      <c r="H54" s="26" t="s">
+      <c r="H54" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="I54" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I54" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="J54" s="28"/>
-      <c r="K54" s="29"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="30"/>
       <c r="L54" s="24"/>
       <c r="M54" s="24"/>
       <c r="N54" s="24"/>
     </row>
     <row r="55" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B55" s="27"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="31"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="32"/>
       <c r="F55" s="24"/>
       <c r="G55" s="24"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="28"/>
-      <c r="J55" s="28"/>
-      <c r="K55" s="29"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="30"/>
       <c r="L55" s="24"/>
       <c r="M55" s="24"/>
       <c r="N55" s="24"/>
@@ -2647,16 +2689,16 @@
       <c r="E56" s="24"/>
       <c r="F56" s="24"/>
       <c r="G56" s="24"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="30"/>
-      <c r="J56" s="30"/>
-      <c r="K56" s="31"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="31"/>
+      <c r="K56" s="32"/>
       <c r="L56" s="24"/>
       <c r="M56" s="24"/>
       <c r="N56" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="49">
     <mergeCell ref="I29:J30"/>
     <mergeCell ref="K29:L30"/>
     <mergeCell ref="M29:M30"/>
@@ -2670,7 +2712,6 @@
     <mergeCell ref="M31:M32"/>
     <mergeCell ref="I33:L35"/>
     <mergeCell ref="M33:M35"/>
-    <mergeCell ref="B34:D34"/>
     <mergeCell ref="H38:M38"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="C39:C40"/>
@@ -2686,9 +2727,9 @@
     <mergeCell ref="C43:E45"/>
     <mergeCell ref="I44:L46"/>
     <mergeCell ref="M44:M46"/>
+    <mergeCell ref="C41:D42"/>
     <mergeCell ref="H50:H51"/>
     <mergeCell ref="I50:I51"/>
-    <mergeCell ref="C41:D42"/>
     <mergeCell ref="E41:E42"/>
     <mergeCell ref="I42:L43"/>
     <mergeCell ref="H54:H56"/>

</xml_diff>